<commit_message>
Updated Exxon importer to get the right units and unit type.
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B117C3-7072-1940-889D-B7A717F735E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F51B7BC-3F00-3549-B5CC-FCFA1D57AAE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="3260" windowWidth="27640" windowHeight="16940" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="1480" yWindow="1640" windowWidth="24100" windowHeight="16960" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -33,9 +33,6 @@
     <t>0.11.0</t>
   </si>
   <si>
-    <t>Metadata:</t>
-  </si>
-  <si>
     <t xml:space="preserve">    API</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t xml:space="preserve">    Alternate Names</t>
   </si>
   <si>
-    <t xml:space="preserve">    Source id</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Name</t>
   </si>
   <si>
@@ -75,20 +69,130 @@
     <t>full reference</t>
   </si>
   <si>
-    <t>Fresh Oil Sample</t>
+    <t xml:space="preserve">    Short name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sample ID</t>
+  </si>
+  <si>
+    <t>Record Metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Boiling Point Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Fraction evaporated</t>
+  </si>
+  <si>
+    <t>Subsample Metadata</t>
+  </si>
+  <si>
+    <t>Physical Properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Density at temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Final Boiling point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Viscosity at temp</t>
+  </si>
+  <si>
+    <t>Distillation Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Pour Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Flash Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Density</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 3</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>Fraction Unit</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Temp Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Type (mass fraction or volume fraction)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Distillation cuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Source ID</t>
+  </si>
+  <si>
+    <t>Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Fraction Recovered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  SARA Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Asphaltenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Resins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Aromatics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Saturates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,8 +215,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,19 +533,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -447,54 +554,54 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -504,7 +611,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -513,9 +620,205 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Physical property data now imported
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BCA4FD-1EF9-864C-8B2C-9DDA45C4A683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED448513-9BCC-7948-9DDE-EC3ECC6476C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="980" windowWidth="32680" windowHeight="17620" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="5320" yWindow="2280" windowWidth="32680" windowHeight="17620" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="152">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -569,12 +569,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -894,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,86 +1129,77 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>26</v>
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" t="s">
-        <v>34</v>
+      <c r="A42" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" t="s">
-        <v>58</v>
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>40</v>
+      <c r="A47" t="s">
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>31</v>
@@ -1217,132 +1207,114 @@
       <c r="C47" t="s">
         <v>32</v>
       </c>
+      <c r="D47" t="s">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" t="s">
-        <v>77</v>
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" t="s">
-        <v>77</v>
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>77</v>
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="E50" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
+      <c r="A52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="C53" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" t="s">
-        <v>47</v>
+      <c r="A55" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C55" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" t="s">
-        <v>48</v>
-      </c>
-      <c r="G55" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" t="s">
         <v>77</v>
       </c>
-      <c r="E56" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" t="s">
-        <v>77</v>
-      </c>
-      <c r="E57" t="s">
-        <v>76</v>
-      </c>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="A58" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" t="s">
         <v>47</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>49</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>32</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>51</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F60" t="s">
         <v>48</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G60" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>142</v>
+        <v>46</v>
       </c>
       <c r="D61" t="s">
         <v>77</v>
@@ -1351,34 +1323,93 @@
         <v>76</v>
       </c>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
+        <v>49</v>
+      </c>
+      <c r="D64" t="s">
+        <v>32</v>
+      </c>
+      <c r="E64" t="s">
+        <v>51</v>
+      </c>
+      <c r="F64" t="s">
+        <v>48</v>
+      </c>
+      <c r="G64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B68" t="s">
         <v>47</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C68" t="s">
         <v>63</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D68" t="s">
         <v>139</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E68" t="s">
         <v>51</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F68" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D69" t="s">
         <v>146</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E69" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1391,12 +1422,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16E494EB-8F6C-C642-91BA-EAB123553603}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E24:E25 E28:E30 E33:E35 E43:E45 C40 D21</xm:sqref>
+          <xm:sqref>E24:E25 E28:E30 D21 E48:E50 C45 E33:E36 E38:E40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
@@ -1408,19 +1439,19 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B33</xm:sqref>
+          <xm:sqref>C33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C48:C51 C43:C45 C41 D20 D56:D57 D60:D61</xm:sqref>
+          <xm:sqref>C53:C56 C48:C50 C46 D20 D61:D62 D65:D66</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$5:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B38 B20 E56:E57 E60:E61</xm:sqref>
+          <xm:sqref>B43 B20 E61:E62 E65:E66</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21D6D9B9-727A-8848-9369-CAA47CDDF88B}">
           <x14:formula1>
@@ -1438,7 +1469,13 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$5:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E64</xm:sqref>
+          <xm:sqref>E69</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59485176-B4F7-C341-8A77-B85A80DCF517}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C38:C40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1473,13 +1510,6 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
@@ -1487,22 +1517,22 @@
       <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1536,7 +1566,7 @@
       <c r="B7" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1559,7 +1589,7 @@
       <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1568,32 +1598,29 @@
       <c r="E8" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="F9" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="F10" s="4" t="s">
+      <c r="F10" t="s">
         <v>80</v>
       </c>
       <c r="H10" t="s">
@@ -1620,53 +1647,53 @@
       <c r="A14" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+      <c r="AB14" s="5"/>
+      <c r="AC14" s="5"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="6"/>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="6"/>
       <c r="AJ14" s="2"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="5"/>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1674,7 +1701,7 @@
       <c r="A16" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1682,7 +1709,7 @@
       <c r="A17" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1690,7 +1717,7 @@
       <c r="A18" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1698,7 +1725,7 @@
       <c r="A19" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1706,7 +1733,7 @@
       <c r="A20" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1714,7 +1741,7 @@
       <c r="A21" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1722,7 +1749,7 @@
       <c r="A22" t="s">
         <v>95</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1730,7 +1757,7 @@
       <c r="A23" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1738,7 +1765,7 @@
       <c r="A24" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1746,7 +1773,7 @@
       <c r="A25" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1754,7 +1781,7 @@
       <c r="A26" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1762,7 +1789,7 @@
       <c r="A27" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1770,7 +1797,7 @@
       <c r="A28" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1778,7 +1805,7 @@
       <c r="A29" t="s">
         <v>102</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1786,7 +1813,7 @@
       <c r="A30" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1794,87 +1821,87 @@
       <c r="A31" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>134</v>
       </c>
     </row>
@@ -1884,27 +1911,27 @@
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="6"/>
+      <c r="B53" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
getting closer to distillation data..
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED448513-9BCC-7948-9DDE-EC3ECC6476C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08439326-83C1-4C44-8DF9-E78DCD9EB2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5320" yWindow="2280" windowWidth="32680" windowHeight="17620" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="1280" yWindow="1580" windowWidth="26900" windowHeight="17460" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
   <si>
-    <t>0.11.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Location Coordinates</t>
   </si>
   <si>
@@ -109,12 +106,6 @@
     <t>Distillation Data</t>
   </si>
   <si>
-    <t xml:space="preserve">  Pour Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Flash Point</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Density</t>
   </si>
   <si>
@@ -169,9 +160,6 @@
     <t xml:space="preserve">  compound 1</t>
   </si>
   <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -451,18 +439,12 @@
     <t xml:space="preserve">  compound 2</t>
   </si>
   <si>
-    <t xml:space="preserve">  Sulphur</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Composition 2</t>
   </si>
   <si>
     <t>Industry Properties</t>
   </si>
   <si>
-    <t xml:space="preserve">Reid Vapor Pressure  </t>
-  </si>
-  <si>
     <t>Pressure</t>
   </si>
   <si>
@@ -482,13 +464,136 @@
   </si>
   <si>
     <t>millibar</t>
+  </si>
+  <si>
+    <t>LSFO</t>
+  </si>
+  <si>
+    <t>VLSFO</t>
+  </si>
+  <si>
+    <t>ULSFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 12</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Reid Vapor Pressure  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Another property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 16</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Interfacial Tension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Seawater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fresh Water</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>N/m</t>
+  </si>
+  <si>
+    <t>mN/m</t>
+  </si>
+  <si>
+    <t>dyn/cm</t>
+  </si>
+  <si>
+    <t>lbf/in</t>
+  </si>
+  <si>
+    <t>erg/cm²</t>
+  </si>
+  <si>
+    <t>erg/mm²</t>
+  </si>
+  <si>
+    <t>j/m²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulfur Content	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waxes	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Composition 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Property 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Property 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Pour Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Flash Point</t>
+  </si>
+  <si>
+    <t>0.12.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -525,28 +630,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -569,16 +663,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,527 +984,747 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
+        <v>184</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>169</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>167</v>
+      </c>
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E28" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>168</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>183</v>
+      </c>
+      <c r="C30" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>26</v>
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" t="s">
-        <v>49</v>
-      </c>
-      <c r="C46" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" t="s">
-        <v>32</v>
-      </c>
-      <c r="D47" t="s">
-        <v>33</v>
-      </c>
-      <c r="E47" t="s">
-        <v>34</v>
+      <c r="A47" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>23</v>
       </c>
-      <c r="E48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>24</v>
-      </c>
-      <c r="E49" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>30</v>
-      </c>
-      <c r="E50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="C54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="C59" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>155</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>157</v>
+      </c>
+      <c r="C64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" t="s">
+        <v>73</v>
+      </c>
+      <c r="E65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" t="s">
+        <v>73</v>
+      </c>
+      <c r="E67" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" t="s">
+        <v>73</v>
+      </c>
+      <c r="E68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B52" t="s">
-        <v>31</v>
-      </c>
-      <c r="C52" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="C72" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B77" t="s">
+        <v>177</v>
+      </c>
+      <c r="C77" t="s">
+        <v>45</v>
+      </c>
+      <c r="D77" t="s">
+        <v>29</v>
+      </c>
+      <c r="E77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" t="s">
         <v>44</v>
       </c>
-      <c r="C53" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="G77" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C54" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
+      <c r="D78" t="s">
+        <v>73</v>
+      </c>
+      <c r="E78" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" t="s">
+        <v>73</v>
+      </c>
+      <c r="E79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B81" t="s">
+        <v>177</v>
+      </c>
+      <c r="C81" t="s">
         <v>45</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D81" t="s">
+        <v>29</v>
+      </c>
+      <c r="E81" t="s">
         <v>47</v>
       </c>
-      <c r="C60" t="s">
-        <v>49</v>
-      </c>
-      <c r="D60" t="s">
-        <v>32</v>
-      </c>
-      <c r="E60" t="s">
-        <v>51</v>
-      </c>
-      <c r="F60" t="s">
-        <v>48</v>
-      </c>
-      <c r="G60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+      <c r="F81" t="s">
+        <v>44</v>
+      </c>
+      <c r="G81" t="s">
         <v>46</v>
       </c>
-      <c r="D61" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B82" t="s">
+        <v>178</v>
+      </c>
+      <c r="D82" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B83" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B85" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D85" t="s">
+        <v>135</v>
+      </c>
+      <c r="E85" t="s">
+        <v>47</v>
+      </c>
+      <c r="F85" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>181</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D86" t="s">
         <v>140</v>
       </c>
-      <c r="D62" t="s">
-        <v>77</v>
-      </c>
-      <c r="E62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" t="s">
-        <v>32</v>
-      </c>
-      <c r="E64" t="s">
-        <v>51</v>
-      </c>
-      <c r="F64" t="s">
-        <v>48</v>
-      </c>
-      <c r="G64" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D65" t="s">
-        <v>77</v>
-      </c>
-      <c r="E65" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D66" t="s">
-        <v>77</v>
-      </c>
-      <c r="E66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B68" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E86" t="s">
         <v>139</v>
       </c>
-      <c r="E68" t="s">
-        <v>51</v>
-      </c>
-      <c r="F68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D69" t="s">
-        <v>146</v>
-      </c>
-      <c r="E69" t="s">
-        <v>145</v>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>182</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{555D19C9-7E2F-7C4E-9874-953E85BB8207}">
       <formula1>20</formula1>
@@ -1422,36 +1733,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16E494EB-8F6C-C642-91BA-EAB123553603}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E24:E25 E28:E30 D21 E48:E50 C45 E33:E36 E38:E40</xm:sqref>
+          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$C$6:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C28:C30</xm:sqref>
+          <xm:sqref>C33:C35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD19B16E-3F59-184B-ACC0-71023DB30176}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C33</xm:sqref>
+          <xm:sqref>C38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C53:C56 C48:C50 C46 D20 D61:D62 D65:D66</xm:sqref>
+          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$5:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B43 B20 E61:E62 E65:E66</xm:sqref>
+          <xm:sqref>B48 B20 E78:E79 E82:E83</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21D6D9B9-727A-8848-9369-CAA47CDDF88B}">
           <x14:formula1>
@@ -1463,19 +1774,31 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$14:$B$52</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:Z11</xm:sqref>
+          <xm:sqref>P11:Z11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A167DD7F-A8F8-B74C-A84A-43543D19A700}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$5:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E69</xm:sqref>
+          <xm:sqref>E86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59485176-B4F7-C341-8A77-B85A80DCF517}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C38:C40</xm:sqref>
+          <xm:sqref>C43:C45</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1912201-6DDE-C248-B538-305BA8FBF0C5}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$B$14:$B$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>B11:O11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD44F0D6-822C-3C42-91E2-D5D29C95944B}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$I$6:$I$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>C28:C30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1485,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
-  <dimension ref="A1:AN53"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="C1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1498,440 +1821,441 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
         <v>76</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B13" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>83</v>
       </c>
-      <c r="H8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="F9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="F10" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="5"/>
-      <c r="W14" s="5"/>
-      <c r="X14" s="5"/>
-      <c r="Y14" s="5"/>
-      <c r="Z14" s="5"/>
-      <c r="AA14" s="5"/>
-      <c r="AB14" s="5"/>
-      <c r="AC14" s="5"/>
-      <c r="AD14" s="5"/>
-      <c r="AE14" s="5"/>
-      <c r="AF14" s="5"/>
-      <c r="AG14" s="6"/>
-      <c r="AH14" s="6"/>
-      <c r="AI14" s="6"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="7"/>
-      <c r="AL14" s="7"/>
-      <c r="AM14" s="5"/>
-      <c r="AN14" s="5"/>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>107</v>
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>108</v>
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>109</v>
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>110</v>
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>113</v>
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>114</v>
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>115</v>
+        <v>94</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>116</v>
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>117</v>
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>118</v>
+        <v>97</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>119</v>
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="5" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="5" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="5" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="5" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="5" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="5" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="5" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="5" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="7" t="s">
+      <c r="B49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="7" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="5" t="s">
-        <v>102</v>
+      <c r="B51" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="5" t="s">
-        <v>103</v>
+      <c r="B52" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="5"/>
+      <c r="B53" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
got compounds and bulk composition done
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7725521-4AFC-794C-A379-6509B04A1D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504194CB-519E-FB4C-83A6-FBAA5239B86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6400" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="188">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t xml:space="preserve">  Distillation Cuts</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
@@ -986,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1596,10 +1599,10 @@
         <v>28</v>
       </c>
       <c r="E77" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F77" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="G77" t="s">
         <v>44</v>
@@ -1612,9 +1615,6 @@
       <c r="D78" t="s">
         <v>71</v>
       </c>
-      <c r="E78" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
@@ -1622,9 +1622,6 @@
       </c>
       <c r="D79" t="s">
         <v>71</v>
-      </c>
-      <c r="E79" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -1762,7 +1759,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$5:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B48 B20 E78:E79 E82:E83</xm:sqref>
+          <xm:sqref>B48 B20 E82:E83</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21D6D9B9-727A-8848-9369-CAA47CDDF88B}">
           <x14:formula1>

</xml_diff>

<commit_message>
a validation error -- hmm
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504194CB-519E-FB4C-83A6-FBAA5239B86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7402A10A-0640-834A-951B-4AF492DA5A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="500" windowWidth="25600" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="7520" yWindow="2520" windowWidth="25600" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -500,9 +500,6 @@
   </si>
   <si>
     <t xml:space="preserve">   Reid Vapor Pressure  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Another property</t>
   </si>
   <si>
     <t xml:space="preserve">    cut 13</t>
@@ -987,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,13 +1006,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>156</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1153,7 +1150,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
         <v>53</v>
@@ -1161,7 +1158,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
@@ -1169,10 +1166,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" t="s">
         <v>59</v>
@@ -1186,10 +1183,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E28" t="s">
         <v>53</v>
@@ -1197,18 +1194,18 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1324,7 +1321,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B50" t="s">
         <v>58</v>
@@ -1346,7 +1343,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B52" t="s">
         <v>27</v>
@@ -1495,7 +1492,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C65" t="s">
         <v>71</v>
@@ -1506,7 +1503,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
         <v>71</v>
@@ -1517,7 +1514,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C67" t="s">
         <v>71</v>
@@ -1528,7 +1525,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C68" t="s">
         <v>71</v>
@@ -1590,7 +1587,7 @@
         <v>40</v>
       </c>
       <c r="B77" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C77" t="s">
         <v>43</v>
@@ -1602,7 +1599,7 @@
         <v>42</v>
       </c>
       <c r="F77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G77" t="s">
         <v>44</v>
@@ -1627,12 +1624,12 @@
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C81" t="s">
         <v>43</v>
@@ -1647,15 +1644,18 @@
         <v>42</v>
       </c>
       <c r="G81" t="s">
+        <v>186</v>
+      </c>
+      <c r="H81" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B82" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D82" t="s">
         <v>71</v>
@@ -1664,12 +1664,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B83" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D83" t="s">
         <v>71</v>
@@ -1678,12 +1678,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>136</v>
       </c>
       <c r="B85" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C85" t="s">
         <v>57</v>
@@ -1698,9 +1698,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>157</v>
@@ -1712,13 +1712,11 @@
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>180</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>158</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="B87" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -1857,7 +1855,7 @@
         <v>137</v>
       </c>
       <c r="I5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1886,7 +1884,7 @@
         <v>138</v>
       </c>
       <c r="I6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1912,7 +1910,7 @@
         <v>139</v>
       </c>
       <c r="I7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1938,7 +1936,7 @@
         <v>140</v>
       </c>
       <c r="I8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1952,7 +1950,7 @@
         <v>141</v>
       </c>
       <c r="I9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1963,7 +1961,7 @@
         <v>143</v>
       </c>
       <c r="I10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1974,12 +1972,12 @@
         <v>142</v>
       </c>
       <c r="I11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adios_db: ECCC import and noaa csv reader
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BCA4FD-1EF9-864C-8B2C-9DDA45C4A683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7402A10A-0640-834A-951B-4AF492DA5A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="980" windowWidth="32680" windowHeight="17620" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="7520" yWindow="2520" windowWidth="25600" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
   <si>
-    <t>0.11.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Location Coordinates</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t xml:space="preserve">    Method</t>
   </si>
   <si>
-    <t xml:space="preserve">    Final Boiling point</t>
-  </si>
-  <si>
     <t xml:space="preserve">    cut 1</t>
   </si>
   <si>
@@ -109,12 +103,6 @@
     <t>Distillation Data</t>
   </si>
   <si>
-    <t xml:space="preserve">  Pour Point</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Flash Point</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Density</t>
   </si>
   <si>
@@ -136,9 +124,6 @@
     <t xml:space="preserve">  Type (mass fraction or volume fraction)</t>
   </si>
   <si>
-    <t xml:space="preserve">  Distillation cuts</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Source ID</t>
   </si>
   <si>
@@ -169,9 +154,6 @@
     <t xml:space="preserve">  compound 1</t>
   </si>
   <si>
-    <t xml:space="preserve">name </t>
-  </si>
-  <si>
     <t>method</t>
   </si>
   <si>
@@ -451,18 +433,12 @@
     <t xml:space="preserve">  compound 2</t>
   </si>
   <si>
-    <t xml:space="preserve">  Sulphur</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Composition 2</t>
   </si>
   <si>
     <t>Industry Properties</t>
   </si>
   <si>
-    <t xml:space="preserve">Reid Vapor Pressure  </t>
-  </si>
-  <si>
     <t>Pressure</t>
   </si>
   <si>
@@ -482,13 +458,142 @@
   </si>
   <si>
     <t>millibar</t>
+  </si>
+  <si>
+    <t>LSFO</t>
+  </si>
+  <si>
+    <t>VLSFO</t>
+  </si>
+  <si>
+    <t>ULSFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 12</t>
+  </si>
+  <si>
+    <t>Template Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Reid Vapor Pressure  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cut 16</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>Interfacial Tension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Seawater</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fresh Water</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>N/m</t>
+  </si>
+  <si>
+    <t>mN/m</t>
+  </si>
+  <si>
+    <t>dyn/cm</t>
+  </si>
+  <si>
+    <t>lbf/in</t>
+  </si>
+  <si>
+    <t>erg/cm²</t>
+  </si>
+  <si>
+    <t>erg/mm²</t>
+  </si>
+  <si>
+    <t>j/m²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sulfur Content	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waxes	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Composition 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Property 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Property 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Pour Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Flash Point</t>
+  </si>
+  <si>
+    <t>0.12.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Final Boiling Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Distillation Cuts</t>
+  </si>
+  <si>
+    <t>comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -525,28 +630,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -569,17 +663,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -894,495 +984,742 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>182</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>164</v>
+      </c>
+      <c r="C28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>165</v>
+      </c>
+      <c r="C29" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>180</v>
+      </c>
+      <c r="C30" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>26</v>
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>49</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>23</v>
       </c>
-      <c r="E43" t="s">
-        <v>58</v>
-      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>30</v>
-      </c>
-      <c r="E45" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>185</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="E53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" t="s">
+        <v>71</v>
+      </c>
+      <c r="E54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="C58" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" t="s">
+        <v>71</v>
+      </c>
+      <c r="E61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+      <c r="C63" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>155</v>
+      </c>
+      <c r="C64" t="s">
+        <v>71</v>
+      </c>
+      <c r="E64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>158</v>
+      </c>
+      <c r="C65" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>159</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>160</v>
+      </c>
+      <c r="C67" t="s">
+        <v>71</v>
+      </c>
+      <c r="E67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" t="s">
+        <v>71</v>
+      </c>
+      <c r="E68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C74" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="B77" t="s">
+        <v>174</v>
+      </c>
+      <c r="C77" t="s">
+        <v>43</v>
+      </c>
+      <c r="D77" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" t="s">
+        <v>42</v>
+      </c>
+      <c r="F77" t="s">
+        <v>186</v>
+      </c>
+      <c r="G77" t="s">
         <v>44</v>
       </c>
-      <c r="C48" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D78" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D79" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B81" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" t="s">
         <v>43</v>
       </c>
-      <c r="C49" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="D81" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" t="s">
+        <v>45</v>
+      </c>
+      <c r="F81" t="s">
         <v>42</v>
       </c>
-      <c r="C50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
+      <c r="G81" t="s">
+        <v>186</v>
+      </c>
+      <c r="H81" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B82" t="s">
+        <v>175</v>
+      </c>
+      <c r="D82" t="s">
+        <v>71</v>
+      </c>
+      <c r="E82" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" t="s">
+        <v>176</v>
+      </c>
+      <c r="D83" t="s">
+        <v>71</v>
+      </c>
+      <c r="E83" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B85" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" t="s">
+        <v>57</v>
+      </c>
+      <c r="D85" t="s">
+        <v>133</v>
+      </c>
+      <c r="E85" t="s">
         <v>45</v>
       </c>
-      <c r="B55" t="s">
-        <v>47</v>
-      </c>
-      <c r="C55" t="s">
-        <v>49</v>
-      </c>
-      <c r="D55" t="s">
-        <v>32</v>
-      </c>
-      <c r="E55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F55" t="s">
-        <v>48</v>
-      </c>
-      <c r="G55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D56" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" t="s">
-        <v>77</v>
-      </c>
-      <c r="E57" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B59" t="s">
-        <v>47</v>
-      </c>
-      <c r="C59" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" t="s">
-        <v>51</v>
-      </c>
-      <c r="F59" t="s">
-        <v>48</v>
-      </c>
-      <c r="G59" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D60" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D61" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B63" t="s">
-        <v>47</v>
-      </c>
-      <c r="C63" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" t="s">
-        <v>139</v>
-      </c>
-      <c r="E63" t="s">
-        <v>51</v>
-      </c>
-      <c r="F63" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D64" t="s">
-        <v>146</v>
-      </c>
-      <c r="E64" t="s">
-        <v>145</v>
-      </c>
+      <c r="F85" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>178</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D86" t="s">
+        <v>138</v>
+      </c>
+      <c r="E86" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>179</v>
+      </c>
+      <c r="B87" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{555D19C9-7E2F-7C4E-9874-953E85BB8207}">
       <formula1>20</formula1>
@@ -1391,36 +1728,36 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16E494EB-8F6C-C642-91BA-EAB123553603}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E24:E25 E28:E30 E33:E35 E43:E45 C40 D21</xm:sqref>
+          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$C$6:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C28:C30</xm:sqref>
+          <xm:sqref>C33:C35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD19B16E-3F59-184B-ACC0-71023DB30176}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B33</xm:sqref>
+          <xm:sqref>C38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C48:C51 C43:C45 C41 D20 D56:D57 D60:D61</xm:sqref>
+          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$5:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B38 B20 E56:E57 E60:E61</xm:sqref>
+          <xm:sqref>B48 B20 E82:E83</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21D6D9B9-727A-8848-9369-CAA47CDDF88B}">
           <x14:formula1>
@@ -1432,13 +1769,31 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$14:$B$52</xm:f>
           </x14:formula1>
-          <xm:sqref>B11:Z11</xm:sqref>
+          <xm:sqref>P11:Z11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A167DD7F-A8F8-B74C-A84A-43543D19A700}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$5:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E64</xm:sqref>
+          <xm:sqref>E86</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{59485176-B4F7-C341-8A77-B85A80DCF517}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>C43:C45</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1912201-6DDE-C248-B538-305BA8FBF0C5}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$B$14:$B$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>B11:O11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD44F0D6-822C-3C42-91E2-D5D29C95944B}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$I$6:$I$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>C28:C30</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1448,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
-  <dimension ref="A1:AN53"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="C1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1461,450 +1816,441 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="B15" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="F10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
-      <c r="AG14" s="7"/>
-      <c r="AH14" s="7"/>
-      <c r="AI14" s="7"/>
-      <c r="AJ14" s="2"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="6"/>
-      <c r="AN14" s="6"/>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>107</v>
+        <v>83</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>108</v>
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>109</v>
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>110</v>
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>111</v>
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>112</v>
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>113</v>
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>114</v>
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>115</v>
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>116</v>
+        <v>93</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>117</v>
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>118</v>
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>119</v>
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>120</v>
+        <v>97</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B31" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="6" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="6" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="6" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="6" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="6" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="6" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="6" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="6" t="s">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="6"/>
+      <c r="B53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>146</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added emulsions to data template
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7402A10A-0640-834A-951B-4AF492DA5A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52FD5E6-DCEE-8845-AF72-63EFC28D5033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="2520" windowWidth="25600" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="2260" yWindow="500" windowWidth="35360" windowHeight="14260" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="204">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -587,6 +587,57 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Environmental Behavior</t>
+  </si>
+  <si>
+    <t>Emulsion Properties</t>
+  </si>
+  <si>
+    <t>Emulsion 1</t>
+  </si>
+  <si>
+    <t>15 °C</t>
+  </si>
+  <si>
+    <t>Visual Stability</t>
+  </si>
+  <si>
+    <t>Unstable</t>
+  </si>
+  <si>
+    <t>Water Content</t>
+  </si>
+  <si>
+    <t>Complex Viscosity</t>
+  </si>
+  <si>
+    <t>Complex Modulus</t>
+  </si>
+  <si>
+    <t>Storage Modulus</t>
+  </si>
+  <si>
+    <t>Loss Modulus</t>
+  </si>
+  <si>
+    <t>Tan Delta (V/E)</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>Mesostable</t>
+  </si>
+  <si>
+    <t>Entrained</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Did not form</t>
   </si>
 </sst>
 </file>
@@ -984,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,6 +1769,88 @@
       </c>
       <c r="B87" s="2"/>
     </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>49</v>
+      </c>
+      <c r="B93" t="s">
+        <v>190</v>
+      </c>
+      <c r="C93" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" t="s">
+        <v>192</v>
+      </c>
+      <c r="C94" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>193</v>
+      </c>
+      <c r="C95" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>194</v>
+      </c>
+      <c r="C96" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>195</v>
+      </c>
+      <c r="C97" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>196</v>
+      </c>
+      <c r="C98" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
@@ -1728,12 +1861,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16E494EB-8F6C-C642-91BA-EAB123553603}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30</xm:sqref>
+          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30 C93</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
@@ -1751,7 +1884,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68</xm:sqref>
+          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68 C95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
@@ -1781,7 +1914,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C43:C45</xm:sqref>
+          <xm:sqref>C43:C45 C96</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1912201-6DDE-C248-B538-305BA8FBF0C5}">
           <x14:formula1>
@@ -1795,6 +1928,18 @@
           </x14:formula1>
           <xm:sqref>C28:C30</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DBD49E76-C41E-9A40-BEE3-0BEF123FC8E4}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$J$6:$J$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>C94</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C79C8E7-C6A7-5347-B5A2-9093B26DF36C}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$H$6:$H$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>C97:C99</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1803,10 +1948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="D1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1819,17 +1964,17 @@
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1857,8 +2002,11 @@
       <c r="I5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1886,8 +2034,11 @@
       <c r="I6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>53</v>
       </c>
@@ -1912,8 +2063,11 @@
       <c r="I7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>54</v>
       </c>
@@ -1938,8 +2092,11 @@
       <c r="I8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>73</v>
       </c>
@@ -1952,8 +2109,11 @@
       <c r="I9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>74</v>
       </c>
@@ -1963,8 +2123,11 @@
       <c r="I10" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -1974,13 +2137,16 @@
       <c r="I11" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
@@ -1988,7 +2154,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -1996,7 +2162,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -2004,7 +2170,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
changed unknown to unknown stability
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52FD5E6-DCEE-8845-AF72-63EFC28D5033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F7C2F5-11F3-0A46-824E-3317C0D61E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="500" windowWidth="35360" windowHeight="14260" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="2260" yWindow="500" windowWidth="35360" windowHeight="14260" activeTab="1" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="205">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -634,10 +634,13 @@
     <t>Entrained</t>
   </si>
   <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>Did not form</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Unknown stability</t>
   </si>
 </sst>
 </file>
@@ -1037,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
   <dimension ref="A1:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView topLeftCell="A90" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1800,9 +1803,6 @@
         <v>191</v>
       </c>
       <c r="B94" t="s">
-        <v>192</v>
-      </c>
-      <c r="C94" t="s">
         <v>199</v>
       </c>
     </row>
@@ -1849,6 +1849,9 @@
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>198</v>
+      </c>
+      <c r="C100" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1932,7 +1935,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$J$6:$J$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C94</xm:sqref>
+          <xm:sqref>B94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C79C8E7-C6A7-5347-B5A2-9093B26DF36C}">
           <x14:formula1>
@@ -1950,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2124,7 +2127,7 @@
         <v>171</v>
       </c>
       <c r="J10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2138,7 +2141,7 @@
         <v>172</v>
       </c>
       <c r="J11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed example NOAA CSV file
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F7C2F5-11F3-0A46-824E-3317C0D61E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDC8245-4DBB-B645-9542-861AD489BC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2260" yWindow="500" windowWidth="35360" windowHeight="14260" activeTab="1" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="3100" yWindow="500" windowWidth="35360" windowHeight="14260" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="208">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -595,36 +595,12 @@
     <t>Emulsion Properties</t>
   </si>
   <si>
-    <t>Emulsion 1</t>
-  </si>
-  <si>
-    <t>15 °C</t>
-  </si>
-  <si>
     <t>Visual Stability</t>
   </si>
   <si>
     <t>Unstable</t>
   </si>
   <si>
-    <t>Water Content</t>
-  </si>
-  <si>
-    <t>Complex Viscosity</t>
-  </si>
-  <si>
-    <t>Complex Modulus</t>
-  </si>
-  <si>
-    <t>Storage Modulus</t>
-  </si>
-  <si>
-    <t>Loss Modulus</t>
-  </si>
-  <si>
-    <t>Tan Delta (V/E)</t>
-  </si>
-  <si>
     <t>Stable</t>
   </si>
   <si>
@@ -641,6 +617,39 @@
   </si>
   <si>
     <t>Unknown stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Emulsion 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Visual Stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Water Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Complex Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Complex Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Storage Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Loss Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Tan Delta (V/E)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kinematic Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Dynamic Viscosity</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H109"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1784,15 +1793,15 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>49</v>
-      </c>
-      <c r="B93" t="s">
-        <v>190</v>
+        <v>198</v>
+      </c>
+      <c r="B93">
+        <v>15</v>
       </c>
       <c r="C93" t="s">
         <v>53</v>
@@ -1800,15 +1809,12 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>191</v>
-      </c>
-      <c r="B94" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C95" t="s">
         <v>43</v>
@@ -1816,42 +1822,106 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C97" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C98" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C99" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="C100" t="s">
-        <v>203</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>206</v>
+      </c>
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" t="s">
+        <v>59</v>
+      </c>
+      <c r="D101" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>207</v>
+      </c>
+      <c r="B106" t="s">
+        <v>33</v>
+      </c>
+      <c r="C106" t="s">
+        <v>59</v>
+      </c>
+      <c r="D106" t="s">
+        <v>29</v>
+      </c>
+      <c r="E106" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +1939,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30 C93</xm:sqref>
+          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30 C93 E102:E105 E107:E109</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
@@ -1881,7 +1951,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C38</xm:sqref>
+          <xm:sqref>C38 C102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
@@ -1917,7 +1987,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C43:C45 C96</xm:sqref>
+          <xm:sqref>C43:C45 C96 C107:C109</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1912201-6DDE-C248-B538-305BA8FBF0C5}">
           <x14:formula1>
@@ -1953,7 +2023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+    <sheetView topLeftCell="A49" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -2006,7 +2076,7 @@
         <v>163</v>
       </c>
       <c r="J5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -2038,7 +2108,7 @@
         <v>167</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -2067,7 +2137,7 @@
         <v>168</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -2096,7 +2166,7 @@
         <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -2113,7 +2183,7 @@
         <v>170</v>
       </c>
       <c r="J9" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -2127,7 +2197,7 @@
         <v>171</v>
       </c>
       <c r="J10" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -2141,7 +2211,7 @@
         <v>172</v>
       </c>
       <c r="J11" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add emulsion to noaa csv reader
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDC8245-4DBB-B645-9542-861AD489BC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B488C10D-1315-3341-B524-DB4685041BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="500" windowWidth="35360" windowHeight="14260" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="2860" yWindow="1960" windowWidth="38700" windowHeight="14840" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="215">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -613,43 +613,64 @@
     <t>Did not form</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Unknown stability</t>
   </si>
   <si>
     <t xml:space="preserve">  Emulsion 1</t>
   </si>
   <si>
-    <t xml:space="preserve">  Temperature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Visual Stability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Water Content</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Complex Viscosity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Complex Modulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Storage Modulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Loss Modulus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Tan Delta (V/E)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kinematic Viscosity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Dynamic Viscosity</t>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>(unitless)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Visual Stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Water Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Complex Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Complex Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Storage Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Loss Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Tan Delta (V/E)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Kinematic Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Viscosity at temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dynamic Viscosity</t>
   </si>
 </sst>
 </file>
@@ -1047,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1793,52 +1814,49 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>198</v>
-      </c>
-      <c r="B93">
-        <v>15</v>
-      </c>
-      <c r="C93" t="s">
-        <v>53</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>199</v>
+        <v>204</v>
+      </c>
+      <c r="C94" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>200</v>
-      </c>
-      <c r="C95" t="s">
-        <v>43</v>
+        <v>205</v>
+      </c>
+      <c r="B95" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C96" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="C97" t="s">
-        <v>139</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="C98" t="s">
         <v>139</v>
@@ -1846,7 +1864,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C99" t="s">
         <v>139</v>
@@ -1854,74 +1872,87 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="C100" t="s">
-        <v>195</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>206</v>
-      </c>
-      <c r="B101" t="s">
-        <v>33</v>
+        <v>211</v>
       </c>
       <c r="C101" t="s">
-        <v>59</v>
-      </c>
-      <c r="D101" t="s">
-        <v>29</v>
-      </c>
-      <c r="E101" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>212</v>
+      </c>
+      <c r="B103" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" t="s">
+        <v>59</v>
+      </c>
+      <c r="D103" t="s">
+        <v>29</v>
+      </c>
+      <c r="E103" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>207</v>
-      </c>
-      <c r="B106" t="s">
-        <v>33</v>
-      </c>
-      <c r="C106" t="s">
-        <v>59</v>
-      </c>
-      <c r="D106" t="s">
-        <v>29</v>
-      </c>
-      <c r="E106" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
-        <v>23</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>33</v>
+      </c>
+      <c r="C108" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108" t="s">
+        <v>29</v>
+      </c>
+      <c r="E108" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1934,12 +1965,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16E494EB-8F6C-C642-91BA-EAB123553603}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30 C93 E102:E105 E107:E109</xm:sqref>
+          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30 C94 E104:E107 E109:E111</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
@@ -1951,13 +1982,13 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C38 C102</xm:sqref>
+          <xm:sqref>C38 C104:C106</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68 C95</xm:sqref>
+          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68 C96</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
@@ -1987,7 +2018,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C43:C45 C96 C107:C109</xm:sqref>
+          <xm:sqref>C43:C45 C97 C109:C111</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1912201-6DDE-C248-B538-305BA8FBF0C5}">
           <x14:formula1>
@@ -2005,13 +2036,19 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$J$6:$J$11</xm:f>
           </x14:formula1>
-          <xm:sqref>B94</xm:sqref>
+          <xm:sqref>B95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C79C8E7-C6A7-5347-B5A2-9093B26DF36C}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$H$6:$H$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C97:C99</xm:sqref>
+          <xm:sqref>C98:C100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60E42108-5C6B-E248-A09B-7B977969C6EC}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$K$6:$K$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>C93</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2021,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="B1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2037,17 +2074,17 @@
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -2078,8 +2115,11 @@
       <c r="J5" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -2110,8 +2150,11 @@
       <c r="J6" s="3" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>53</v>
       </c>
@@ -2139,8 +2182,11 @@
       <c r="J7" s="3" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>54</v>
       </c>
@@ -2168,8 +2214,11 @@
       <c r="J8" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>73</v>
       </c>
@@ -2185,8 +2234,11 @@
       <c r="J9" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>74</v>
       </c>
@@ -2200,7 +2252,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -2211,15 +2263,15 @@
         <v>172</v>
       </c>
       <c r="J11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
@@ -2227,7 +2279,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -2235,7 +2287,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -2243,7 +2295,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>83</v>
       </c>

</xml_diff>

<commit_message>
Merge the Node 18 upgrade changes
</commit_message>
<xml_diff>
--- a/adios_db/data/ADIOS_data_template.xlsx
+++ b/adios_db/data/ADIOS_data_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7402A10A-0640-834A-951B-4AF492DA5A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B488C10D-1315-3341-B524-DB4685041BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="2520" windowWidth="25600" windowHeight="14400" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="2860" yWindow="1960" windowWidth="38700" windowHeight="14840" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="215">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -587,6 +587,90 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>Environmental Behavior</t>
+  </si>
+  <si>
+    <t>Emulsion Properties</t>
+  </si>
+  <si>
+    <t>Visual Stability</t>
+  </si>
+  <si>
+    <t>Unstable</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>Mesostable</t>
+  </si>
+  <si>
+    <t>Entrained</t>
+  </si>
+  <si>
+    <t>Did not form</t>
+  </si>
+  <si>
+    <t>Unknown stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Emulsion 1</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>second</t>
+  </si>
+  <si>
+    <t>(unitless)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Visual Stability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Water Content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Complex Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Complex Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Storage Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Loss Modulus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Tan Delta (V/E)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Kinematic Viscosity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Viscosity at temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dynamic Viscosity</t>
   </si>
 </sst>
 </file>
@@ -984,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="161" zoomScaleNormal="161" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="E106" sqref="E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,6 +1802,159 @@
       </c>
       <c r="B87" s="2"/>
     </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>204</v>
+      </c>
+      <c r="C94" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>205</v>
+      </c>
+      <c r="B95" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>206</v>
+      </c>
+      <c r="C96" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>207</v>
+      </c>
+      <c r="C97" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>208</v>
+      </c>
+      <c r="C98" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>209</v>
+      </c>
+      <c r="C99" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>210</v>
+      </c>
+      <c r="C100" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>211</v>
+      </c>
+      <c r="C101" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>212</v>
+      </c>
+      <c r="B103" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" t="s">
+        <v>59</v>
+      </c>
+      <c r="D103" t="s">
+        <v>29</v>
+      </c>
+      <c r="E103" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>33</v>
+      </c>
+      <c r="C108" t="s">
+        <v>59</v>
+      </c>
+      <c r="D108" t="s">
+        <v>29</v>
+      </c>
+      <c r="E108" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>213</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">
@@ -1728,12 +1965,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16E494EB-8F6C-C642-91BA-EAB123553603}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30</xm:sqref>
+          <xm:sqref>E53:E68 E33:E35 D21 C50 E38:E41 E43:E45 E24:E26 E28:E30 C94 E104:E107 E109:E111</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
@@ -1745,13 +1982,13 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C38</xm:sqref>
+          <xm:sqref>C38 C104:C106</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68</xm:sqref>
+          <xm:sqref>C71:C74 D82:D83 C51 D20 D78:D79 C53:C68 C96</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
@@ -1781,7 +2018,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$E$6:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C43:C45</xm:sqref>
+          <xm:sqref>C43:C45 C97 C109:C111</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B1912201-6DDE-C248-B538-305BA8FBF0C5}">
           <x14:formula1>
@@ -1795,6 +2032,24 @@
           </x14:formula1>
           <xm:sqref>C28:C30</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DBD49E76-C41E-9A40-BEE3-0BEF123FC8E4}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$J$6:$J$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B95</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C79C8E7-C6A7-5347-B5A2-9093B26DF36C}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$H$6:$H$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>C98:C100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60E42108-5C6B-E248-A09B-7B977969C6EC}">
+          <x14:formula1>
+            <xm:f>'Pick List Data'!$K$6:$K$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>C93</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1803,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E050F40-439B-F84D-84F4-6A0869532376}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="B1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1819,17 +2074,17 @@
     <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1857,8 +2112,14 @@
       <c r="I5" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>189</v>
+      </c>
+      <c r="K5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1886,8 +2147,14 @@
       <c r="I6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>53</v>
       </c>
@@ -1912,8 +2179,14 @@
       <c r="I7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>54</v>
       </c>
@@ -1938,8 +2211,14 @@
       <c r="I8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>190</v>
+      </c>
+      <c r="K8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F9" t="s">
         <v>73</v>
       </c>
@@ -1952,8 +2231,14 @@
       <c r="I9" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>193</v>
+      </c>
+      <c r="K9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>74</v>
       </c>
@@ -1963,8 +2248,11 @@
       <c r="I10" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -1974,13 +2262,16 @@
       <c r="I11" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
@@ -1988,7 +2279,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -1996,7 +2287,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>82</v>
       </c>
@@ -2004,7 +2295,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>83</v>
       </c>

</xml_diff>